<commit_message>
Added check e-mail box
</commit_message>
<xml_diff>
--- a/site_check-list.xlsx
+++ b/site_check-list.xlsx
@@ -157,7 +157,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="348" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="353" uniqueCount="117">
   <si>
     <t>Brouser</t>
   </si>
@@ -801,6 +801,37 @@
   </si>
   <si>
     <t>4.10</t>
+  </si>
+  <si>
+    <t>4.11</t>
+  </si>
+  <si>
+    <r>
+      <t xml:space="preserve">check e-mail box which was introduced in step  </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">4.3. </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Calibri"/>
+        <family val="2"/>
+        <charset val="204"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>Must receive a letter to the specified box with the details of the payment order</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -896,7 +927,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="11">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -1050,11 +1081,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thick">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1109,12 +1153,81 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Обычный" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -1134,7 +1247,7 @@
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
       <a:lt1>
-        <a:sysClr val="window" lastClr="FFFFFF"/>
+        <a:sysClr val="window" lastClr="F6F6F6"/>
       </a:lt1>
       <a:dk2>
         <a:srgbClr val="44546A"/>
@@ -2226,10 +2339,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F34"/>
+  <dimension ref="A1:F35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B37" sqref="B37"/>
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2779,14 +2892,14 @@
       </c>
       <c r="F32" s="9"/>
     </row>
-    <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A33" s="17" t="s">
+    <row r="33" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A33" s="10" t="s">
         <v>114</v>
       </c>
-      <c r="B33" s="23" t="s">
+      <c r="B33" t="s">
         <v>113</v>
       </c>
-      <c r="C33" s="19" t="s">
+      <c r="C33" s="12" t="s">
         <v>17</v>
       </c>
       <c r="D33" s="12" t="s">
@@ -2795,10 +2908,29 @@
       <c r="E33" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="F33" s="20"/>
-    </row>
-    <row r="34" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
+      <c r="F33" s="24"/>
+    </row>
+    <row r="34" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A34" s="17" t="s">
+        <v>115</v>
+      </c>
+      <c r="B34" s="23" t="s">
+        <v>116</v>
+      </c>
+      <c r="C34" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D34" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="E34" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="F34" s="20"/>
+    </row>
+    <row r="35" spans="1:6" ht="15.75" thickTop="1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" verticalDpi="0" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>